<commit_message>
UI fix: wider black-screen to eliminate white strip on right
</commit_message>
<xml_diff>
--- a/db/RC1_punchlist_v7.xlsx
+++ b/db/RC1_punchlist_v7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="600" windowWidth="24960" windowHeight="16800" tabRatio="500"/>
+    <workbookView xWindow="1160" yWindow="220" windowWidth="19460" windowHeight="12600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="104">
+  <si>
+    <t>Insert LTL trucking and latex-free icons on product page templates</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>Wound Care/ Woiund Management / Dressings: OpSite Dressing (790042)</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -43,6 +47,38 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>fixed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ys</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gauze sponges xx0049, ..51, …52 but NOT …50</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>22 of 42. Of these, 5 not doable; another 3 waiting images; so 22 of 34 possible, ~70%</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LL Category page template: increase height of product boxes to accommodate 3-line product names; in views/categories/show.html.erb — move to a .css file?</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>— Change clipping of product name in views/categories/show.html.erb from 37 to 40 characters to take advantage of the 3rd line</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>— Check for cases in which a single word is longer than a row</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>Consolidate Formfit Wrist Brace in Orthopedics/Hand &amp; Wrist 750103- (8”) &amp; 750104- (6”) together. Put additional bullet to read Offered in both 6” and 8” models</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -59,23 +95,11 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>no</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Take out NPWT Canister &amp; NPWT Non-Canister from Wound Care</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>— Check for cases in which a single word is longer than a row</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>done</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gauze sponges xx0049, ..51, …52 but NOT …50</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -173,15 +197,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>no</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>fixed</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>no</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -291,14 +307,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>LL Category page template: increase height of product boxes to accommodate 3-line product names; in views/categories/show.html.erb — move to a .css file?</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>— Change clipping of product name in views/categories/show.html.erb from 37 to 40 characters to take advantage of the 3rd line</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>twfar</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -394,10 +402,6 @@
   </si>
   <si>
     <t>no</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Insert LTL trucking and latex-free icons on product page templates</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -994,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:Q67"/>
+  <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:XFD61"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1013,49 +1017,49 @@
   <sheetData>
     <row r="1" spans="1:12" ht="26">
       <c r="A1" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="K2" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="K3" s="13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="E4" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1066,10 +1070,10 @@
         <v>39536</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="8"/>
@@ -1078,7 +1082,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1089,10 +1093,10 @@
         <v>39536</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
@@ -1102,25 +1106,31 @@
         <v>2</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="11">
+      <c r="A7" s="7">
         <v>39535</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="B7" s="7">
+        <v>39537</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="10">
+      <c r="H7" s="8">
         <f t="shared" ref="H7:H13" si="0">H6+1</f>
         <v>3</v>
       </c>
-      <c r="I7" s="10" t="s">
-        <v>91</v>
+      <c r="I7" s="8" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1129,10 +1139,10 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>74</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="4"/>
@@ -1142,19 +1152,19 @@
         <v>4</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="2">
-        <v>39537</v>
+      <c r="A9" s="11">
+        <v>39535</v>
       </c>
       <c r="H9" s="10">
         <f t="shared" ref="H9:H13" si="1">H8+1</f>
         <v>5</v>
       </c>
-      <c r="I9" t="s">
-        <v>75</v>
+      <c r="I9" s="10" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1162,14 +1172,14 @@
         <v>39536</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H10" s="12">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1177,14 +1187,14 @@
         <v>39536</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H11" s="12">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1192,14 +1202,14 @@
         <v>39536</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H12" s="12">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1211,75 +1221,75 @@
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="2">
+      <c r="A14" s="5">
         <v>39537</v>
       </c>
       <c r="B14" s="7">
         <v>39537</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G14" s="8"/>
-      <c r="H14" s="8">
+      <c r="H14" s="4">
         <v>10</v>
       </c>
-      <c r="I14" s="8" t="s">
-        <v>48</v>
+      <c r="I14" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="7">
+      <c r="A15" s="5">
         <v>39537</v>
       </c>
       <c r="B15" s="7">
         <v>39537</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8" t="s">
-        <v>49</v>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="2"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="10" t="s">
-        <v>9</v>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="2"/>
       <c r="E17" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="2"/>
       <c r="G19" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1290,10 +1300,10 @@
         <v>39537</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1303,7 +1313,7 @@
         <v>11</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1314,17 +1324,17 @@
         <v>39537</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" t="s">
-        <v>28</v>
+        <v>85</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="H21" s="21">
         <f>H20+1</f>
         <v>12</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1341,20 +1351,20 @@
         <v>13</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="2"/>
       <c r="C23" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" t="s">
-        <v>28</v>
+        <v>85</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="23" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="20"/>
@@ -1364,24 +1374,24 @@
     <row r="24" spans="1:17">
       <c r="A24" s="2"/>
       <c r="C24" s="12" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="25" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="2"/>
       <c r="C25" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" t="s">
-        <v>28</v>
+        <v>85</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="H25" s="22"/>
       <c r="I25" s="23" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1389,14 +1399,14 @@
         <v>39536</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H26" s="16">
         <f>H22+1</f>
         <v>14</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1407,17 +1417,17 @@
         <v>39537</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H27" s="18">
         <f>H26+1</f>
         <v>15</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="20"/>
@@ -1437,7 +1447,7 @@
         <v>16</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -1449,7 +1459,7 @@
         <v>17</v>
       </c>
       <c r="I29" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -1461,7 +1471,7 @@
         <v>18</v>
       </c>
       <c r="I30" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -1474,82 +1484,82 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31">
+      <c r="H31" s="4">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:17" s="4" customFormat="1">
-      <c r="A32" s="7">
+      <c r="A32" s="5">
         <v>39537</v>
       </c>
       <c r="B32" s="7">
         <v>39537</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="H32" s="4">
         <f>H31+1</f>
         <v>20</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="K32" s="26"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="7">
+      <c r="A33" s="5">
         <v>39537</v>
       </c>
       <c r="B33" s="7">
         <v>39537</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="8">
+      <c r="H33" s="4">
         <f>H32+1</f>
         <v>21</v>
       </c>
-      <c r="I33" s="8" t="s">
-        <v>14</v>
+      <c r="I33" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="7">
+      <c r="A34" s="5">
         <v>39537</v>
       </c>
       <c r="B34" s="7">
         <v>39537</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="8">
+      <c r="H34" s="4">
         <f>H33+1</f>
         <v>22</v>
       </c>
-      <c r="I34" s="8" t="s">
-        <v>18</v>
+      <c r="I34" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1560,10 +1570,10 @@
         <v>39537</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -1573,7 +1583,7 @@
         <v>23</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1582,7 +1592,7 @@
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -1593,7 +1603,7 @@
         <v>24</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1610,7 +1620,7 @@
     <row r="38" spans="1:10">
       <c r="A38" s="2"/>
       <c r="G38" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1625,7 +1635,7 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J39" s="8"/>
     </row>
@@ -1635,10 +1645,10 @@
         <v>39537</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
@@ -1648,7 +1658,7 @@
         <v>25</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J40" s="8"/>
     </row>
@@ -1658,10 +1668,10 @@
         <v>39537</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
@@ -1671,7 +1681,7 @@
         <v>26</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J41" s="8"/>
     </row>
@@ -1681,17 +1691,17 @@
         <v>39537</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J42" s="8"/>
     </row>
@@ -1701,10 +1711,10 @@
         <v>39537</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
@@ -1714,7 +1724,7 @@
         <v>27</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J43" s="8"/>
     </row>
@@ -1724,10 +1734,10 @@
         <v>39537</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -1737,7 +1747,7 @@
         <v>28</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J44" s="8"/>
     </row>
@@ -1747,10 +1757,10 @@
         <v>39537</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
@@ -1760,32 +1770,32 @@
         <v>29</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J45" s="8"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="7">
+      <c r="A46" s="5">
         <v>39537</v>
       </c>
       <c r="B46" s="7">
         <v>39537</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="8">
+      <c r="H46" s="4">
         <f>H45+1</f>
         <v>30</v>
       </c>
-      <c r="I46" s="8" t="s">
-        <v>71</v>
+      <c r="I46" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="J46" s="8"/>
     </row>
@@ -1797,17 +1807,17 @@
         <v>39537</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H47" s="8">
         <f>H46+1</f>
         <v>31</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -1821,7 +1831,7 @@
     <row r="50" spans="1:13">
       <c r="A50" s="2"/>
       <c r="F50" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -1834,7 +1844,7 @@
         <v>32</v>
       </c>
       <c r="I51" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -1843,7 +1853,7 @@
     <row r="53" spans="1:13">
       <c r="A53" s="2"/>
       <c r="F53" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G53" s="1"/>
     </row>
@@ -1852,14 +1862,14 @@
         <v>39536</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H54" s="14">
         <f>H51+1</f>
         <v>33</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J54" s="14"/>
       <c r="K54" s="15"/>
@@ -1874,17 +1884,17 @@
         <v>39537</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="H55" s="8">
         <f>H54+1</f>
         <v>34</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="K55" s="20"/>
     </row>
@@ -1893,14 +1903,14 @@
         <v>39536</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H56" s="14">
         <f t="shared" ref="H56:H57" si="4">H55+1</f>
         <v>35</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J56" s="14"/>
       <c r="K56" s="15"/>
@@ -1915,17 +1925,17 @@
         <v>39537</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="H57" s="8">
         <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="K57" s="20"/>
     </row>
@@ -1937,10 +1947,10 @@
         <v>39537</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
@@ -1950,55 +1960,55 @@
         <v>37</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="7">
+      <c r="A59" s="5">
         <v>39537</v>
       </c>
       <c r="B59" s="7">
         <v>39537</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
-      <c r="H59" s="8">
+      <c r="H59" s="4">
         <f>H58+1</f>
         <v>38</v>
       </c>
-      <c r="I59" s="8" t="s">
-        <v>11</v>
+      <c r="I59" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="7">
+      <c r="A60" s="5">
         <v>39537</v>
       </c>
       <c r="B60" s="7">
         <v>39537</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
-      <c r="H60" s="8">
+      <c r="H60" s="4">
         <f>H59+1</f>
         <v>39</v>
       </c>
-      <c r="I60" s="8" t="s">
-        <v>2</v>
+      <c r="I60" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -2015,7 +2025,7 @@
     <row r="62" spans="1:13">
       <c r="A62" s="2"/>
       <c r="F62" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -2028,7 +2038,7 @@
         <v>40</v>
       </c>
       <c r="I63" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -2037,7 +2047,7 @@
     <row r="65" spans="1:9">
       <c r="A65" s="2"/>
       <c r="E65" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2049,7 +2059,7 @@
         <v>41</v>
       </c>
       <c r="I66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2061,7 +2071,12 @@
         <v>42</v>
       </c>
       <c r="I67" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="H69" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Layout: added 'Home' button to header
</commit_message>
<xml_diff>
--- a/db/RC1_punchlist_v7.xlsx
+++ b/db/RC1_punchlist_v7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="220" windowWidth="19460" windowHeight="12600" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="120" windowWidth="22780" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="106">
   <si>
     <t>Insert LTL trucking and latex-free icons on product page templates</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>missing image:750178</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>missing image:750124</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>missing image: 790064</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need Home button at top area.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>added</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>24 of 42. Of these, 5 not doable; another 3 waiting images; so 24 of 34 possible, =70%</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -63,10 +87,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>22 of 42. Of these, 5 not doable; another 3 waiting images; so 22 of 34 possible, ~70%</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>LL Category page template: increase height of product boxes to accommodate 3-line product names; in views/categories/show.html.erb — move to a .css file?</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -185,10 +205,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>missing 1 image</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">(2) we are missing the image for 750124-000 </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -241,10 +257,6 @@
       </rPr>
       <t xml:space="preserve">Yes. We don't have this image. </t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>missing image</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -469,10 +481,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Need Home button at top area.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Mandy will provide additional pics for Quantum fitness equipment</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -521,7 +529,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -559,6 +567,11 @@
       <b/>
       <sz val="10"/>
       <color indexed="57"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="17"/>
       <name val="Verdana"/>
     </font>
     <font>
@@ -631,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -645,13 +658,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -664,8 +678,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1001,7 +1015,7 @@
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1012,54 +1026,54 @@
     <col min="6" max="6" width="3.5703125" customWidth="1"/>
     <col min="7" max="7" width="2" customWidth="1"/>
     <col min="8" max="8" width="2.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="13"/>
+    <col min="11" max="11" width="10.7109375" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26">
       <c r="A1" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>62</v>
+        <v>104</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" t="s">
         <v>63</v>
       </c>
-      <c r="L2" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" t="s">
         <v>64</v>
-      </c>
-      <c r="L3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="E4" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1070,10 +1084,10 @@
         <v>39536</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="8"/>
@@ -1082,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1093,10 +1107,10 @@
         <v>39536</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
@@ -1106,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1117,10 +1131,10 @@
         <v>39537</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="4"/>
@@ -1130,19 +1144,19 @@
         <v>3</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="11">
+      <c r="A8" s="12">
         <v>39535</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="4"/>
@@ -1152,11 +1166,11 @@
         <v>4</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="11">
+      <c r="A9" s="12">
         <v>39535</v>
       </c>
       <c r="H9" s="10">
@@ -1171,57 +1185,69 @@
       <c r="A10" s="2">
         <v>39536</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="12">
+      <c r="C10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="13">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>54</v>
+      <c r="I10" s="13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="2">
         <v>39536</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="12">
+      <c r="C11" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="13">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>55</v>
+      <c r="I11" s="13" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2">
         <v>39536</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="12">
+      <c r="C12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="13">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I12" s="12" t="s">
-        <v>56</v>
+      <c r="I12" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="2">
-        <v>39536</v>
-      </c>
-      <c r="H13" s="10">
+      <c r="A13" s="7">
+        <v>39536</v>
+      </c>
+      <c r="B13" s="7">
+        <v>39537</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="8">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I13" t="s">
-        <v>93</v>
+      <c r="I13" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1232,17 +1258,17 @@
         <v>39537</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="4">
         <v>10</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1253,16 +1279,16 @@
         <v>39537</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1270,26 +1296,26 @@
       <c r="G16" s="8"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="2"/>
       <c r="E17" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="2"/>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1300,20 +1326,20 @@
         <v>39537</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="18">
+      <c r="H20" s="19">
         <f>H14+1</f>
         <v>11</v>
       </c>
-      <c r="I20" s="19" t="s">
-        <v>48</v>
+      <c r="I20" s="20" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1324,17 +1350,17 @@
         <v>39537</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H21" s="21">
+        <v>78</v>
+      </c>
+      <c r="H21" s="22">
         <f>H20+1</f>
         <v>12</v>
       </c>
-      <c r="I21" s="19" t="s">
-        <v>37</v>
+      <c r="I21" s="20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1346,67 +1372,67 @@
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="H22" s="16">
+      <c r="H22" s="17">
         <f>H21+1</f>
         <v>13</v>
       </c>
-      <c r="I22" s="24" t="s">
-        <v>27</v>
+      <c r="I22" s="25" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="2"/>
       <c r="C23" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H23" s="22"/>
-      <c r="I23" s="23" t="s">
-        <v>38</v>
+        <v>78</v>
+      </c>
+      <c r="H23" s="23"/>
+      <c r="I23" s="24" t="s">
+        <v>42</v>
       </c>
       <c r="J23" s="8"/>
-      <c r="K23" s="20"/>
+      <c r="K23" s="21"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="2"/>
-      <c r="C24" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="25" t="s">
-        <v>32</v>
+      <c r="C24" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="23"/>
+      <c r="I24" s="26" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="2"/>
       <c r="C25" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" s="22"/>
-      <c r="I25" s="23" t="s">
-        <v>33</v>
+        <v>78</v>
+      </c>
+      <c r="H25" s="23"/>
+      <c r="I25" s="24" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="2">
         <v>39536</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H26" s="16">
+      <c r="C26" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" s="17">
         <f>H22+1</f>
         <v>14</v>
       </c>
-      <c r="I26" s="17" t="s">
-        <v>40</v>
+      <c r="I26" s="18" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1417,20 +1443,20 @@
         <v>39537</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H27" s="18">
+        <v>78</v>
+      </c>
+      <c r="H27" s="19">
         <f>H26+1</f>
         <v>15</v>
       </c>
-      <c r="I27" s="19" t="s">
-        <v>39</v>
+      <c r="I27" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="J27" s="8"/>
-      <c r="K27" s="20"/>
+      <c r="K27" s="21"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
@@ -1446,8 +1472,8 @@
         <f t="shared" ref="H28" si="2">H27+1</f>
         <v>16</v>
       </c>
-      <c r="I28" s="17" t="s">
-        <v>94</v>
+      <c r="I28" s="18" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -1459,7 +1485,7 @@
         <v>17</v>
       </c>
       <c r="I29" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -1471,7 +1497,7 @@
         <v>18</v>
       </c>
       <c r="I30" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -1489,7 +1515,7 @@
         <v>19</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:17" s="4" customFormat="1">
@@ -1500,19 +1526,19 @@
         <v>39537</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H32" s="4">
         <f>H31+1</f>
         <v>20</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K32" s="26"/>
+        <v>39</v>
+      </c>
+      <c r="K32" s="27"/>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="5">
@@ -1522,10 +1548,10 @@
         <v>39537</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -1535,7 +1561,7 @@
         <v>21</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1546,10 +1572,10 @@
         <v>39537</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -1559,7 +1585,7 @@
         <v>22</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1570,10 +1596,10 @@
         <v>39537</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -1583,7 +1609,7 @@
         <v>23</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1591,8 +1617,8 @@
         <v>39537</v>
       </c>
       <c r="B36" s="4"/>
-      <c r="C36" s="12" t="s">
-        <v>41</v>
+      <c r="C36" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -1602,25 +1628,25 @@
         <f>H35+1</f>
         <v>24</v>
       </c>
-      <c r="I36" s="12" t="s">
-        <v>2</v>
+      <c r="I36" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="5"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="12"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="8"/>
-      <c r="I37" s="12"/>
+      <c r="I37" s="13"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="2"/>
       <c r="G38" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1635,7 +1661,7 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J39" s="8"/>
     </row>
@@ -1645,10 +1671,10 @@
         <v>39537</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
@@ -1658,7 +1684,7 @@
         <v>25</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J40" s="8"/>
     </row>
@@ -1668,10 +1694,10 @@
         <v>39537</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
@@ -1681,7 +1707,7 @@
         <v>26</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J41" s="8"/>
     </row>
@@ -1691,17 +1717,17 @@
         <v>39537</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J42" s="8"/>
     </row>
@@ -1711,10 +1737,10 @@
         <v>39537</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
@@ -1724,7 +1750,7 @@
         <v>27</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J43" s="8"/>
     </row>
@@ -1734,10 +1760,10 @@
         <v>39537</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -1747,7 +1773,7 @@
         <v>28</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J44" s="8"/>
     </row>
@@ -1757,10 +1783,10 @@
         <v>39537</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
@@ -1770,7 +1796,7 @@
         <v>29</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="J45" s="8"/>
     </row>
@@ -1782,10 +1808,10 @@
         <v>39537</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
@@ -1795,7 +1821,7 @@
         <v>30</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="J46" s="8"/>
     </row>
@@ -1807,17 +1833,17 @@
         <v>39537</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H47" s="8">
         <f>H46+1</f>
         <v>31</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -1831,7 +1857,7 @@
     <row r="50" spans="1:13">
       <c r="A50" s="2"/>
       <c r="F50" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -1844,7 +1870,7 @@
         <v>32</v>
       </c>
       <c r="I51" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -1853,7 +1879,7 @@
     <row r="53" spans="1:13">
       <c r="A53" s="2"/>
       <c r="F53" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G53" s="1"/>
     </row>
@@ -1861,20 +1887,20 @@
       <c r="A54" s="2">
         <v>39536</v>
       </c>
-      <c r="C54" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="H54" s="14">
+      <c r="C54" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H54" s="15">
         <f>H51+1</f>
         <v>33</v>
       </c>
-      <c r="I54" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="J54" s="14"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
+      <c r="I54" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J54" s="15"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
     </row>
     <row r="55" spans="1:13" s="8" customFormat="1">
       <c r="A55" s="7">
@@ -1884,38 +1910,38 @@
         <v>39537</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H55" s="8">
         <f>H54+1</f>
         <v>34</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K55" s="20"/>
+        <v>17</v>
+      </c>
+      <c r="K55" s="21"/>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="2">
         <v>39536</v>
       </c>
-      <c r="C56" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="H56" s="14">
+      <c r="C56" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H56" s="15">
         <f t="shared" ref="H56:H57" si="4">H55+1</f>
         <v>35</v>
       </c>
-      <c r="I56" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J56" s="14"/>
-      <c r="K56" s="15"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
+      <c r="I56" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J56" s="15"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="15"/>
     </row>
     <row r="57" spans="1:13" s="8" customFormat="1">
       <c r="A57" s="7">
@@ -1925,19 +1951,19 @@
         <v>39537</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H57" s="8">
         <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K57" s="20"/>
+        <v>19</v>
+      </c>
+      <c r="K57" s="21"/>
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="7">
@@ -1947,10 +1973,10 @@
         <v>39537</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
@@ -1960,7 +1986,7 @@
         <v>37</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -1971,10 +1997,10 @@
         <v>39537</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
@@ -1984,7 +2010,7 @@
         <v>38</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -1995,10 +2021,10 @@
         <v>39537</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
@@ -2008,7 +2034,7 @@
         <v>39</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -2025,7 +2051,7 @@
     <row r="62" spans="1:13">
       <c r="A62" s="2"/>
       <c r="F62" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -2038,7 +2064,7 @@
         <v>40</v>
       </c>
       <c r="I63" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -2047,7 +2073,7 @@
     <row r="65" spans="1:9">
       <c r="A65" s="2"/>
       <c r="E65" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2059,7 +2085,7 @@
         <v>41</v>
       </c>
       <c r="I66" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2071,15 +2097,16 @@
         <v>42</v>
       </c>
       <c r="I67" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="H69" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>